<commit_message>
added ability to derive row attributes/columns from spreadsheet
</commit_message>
<xml_diff>
--- a/test3.xlsx
+++ b/test3.xlsx
@@ -4,26 +4,148 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="test7" sheetId="5" r:id="rId1"/>
+    <sheet name="test8" sheetId="6" r:id="rId2"/>
+    <sheet name="test9" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
   <si>
     <t>blah7</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,13 +153,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,8 +188,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,16 +497,320 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added ability to automatically find cell range of worksheet
</commit_message>
<xml_diff>
--- a/test3.xlsx
+++ b/test3.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="test7" sheetId="5" r:id="rId1"/>
     <sheet name="test8" sheetId="6" r:id="rId2"/>
     <sheet name="test9" sheetId="7" r:id="rId3"/>
+    <sheet name="test10" sheetId="8" r:id="rId4"/>
+    <sheet name="test11" sheetId="9" r:id="rId5"/>
+    <sheet name="test12" sheetId="10" r:id="rId6"/>
+    <sheet name="test13" sheetId="11" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="45">
   <si>
     <t>A1</t>
   </si>
@@ -139,6 +143,18 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>blah10</t>
+  </si>
+  <si>
+    <t>blah11</t>
+  </si>
+  <si>
+    <t>blah12</t>
+  </si>
+  <si>
+    <t>blah13</t>
   </si>
 </sst>
 </file>
@@ -667,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -813,4 +829,612 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:P4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>